<commit_message>
#6 - Replaced the 5V reference with a resistor divider. It should give a voltage of 5.1V.
</commit_message>
<xml_diff>
--- a/bom/schraeg_BOM.xlsx
+++ b/bom/schraeg_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="172">
   <si>
     <t xml:space="preserve">SCHRÄG, v0.2.2</t>
   </si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">603-CC0603MR9BB104</t>
   </si>
   <si>
-    <t xml:space="preserve">C14,C18</t>
+    <t xml:space="preserve">C18</t>
   </si>
   <si>
     <t xml:space="preserve">220n</t>
@@ -196,7 +196,7 @@
     <t xml:space="preserve">771-BZT52-C4V7X</t>
   </si>
   <si>
-    <t xml:space="preserve">D4,D6</t>
+    <t xml:space="preserve">D6</t>
   </si>
   <si>
     <t xml:space="preserve">Voltage reference</t>
@@ -250,12 +250,72 @@
     <t xml:space="preserve">652-MF-NSMF050-2</t>
   </si>
   <si>
+    <t xml:space="preserve">R15,R30,R32,R39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor, 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF4700V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF4700V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R23,R24,R25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF1001V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF1001V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1K5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF1501V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF1501V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6K8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF6801V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF6801V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF1002V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF1002V</t>
+  </si>
+  <si>
     <t xml:space="preserve">R14,R40</t>
   </si>
   <si>
-    <t xml:space="preserve">Resistor, 1%</t>
-  </si>
-  <si>
     <t xml:space="preserve">15K</t>
   </si>
   <si>
@@ -265,18 +325,6 @@
     <t xml:space="preserve">667-ERJ-3EKF1502V</t>
   </si>
   <si>
-    <t xml:space="preserve">R15,R30,R32,R39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">470R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF4700V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF4700V</t>
-  </si>
-  <si>
     <t xml:space="preserve">R18</t>
   </si>
   <si>
@@ -289,6 +337,18 @@
     <t xml:space="preserve">667-ERJ-3EKF2202V</t>
   </si>
   <si>
+    <t xml:space="preserve">R27,R28,R29,R31,R33,R34,R35,R36,R38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF3302V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF3302V</t>
+  </si>
+  <si>
     <t xml:space="preserve">R2,R5,R19,R22,R48</t>
   </si>
   <si>
@@ -301,28 +361,28 @@
     <t xml:space="preserve">667-ERJ-3EKF4702V</t>
   </si>
   <si>
-    <t xml:space="preserve">R21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF1002V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF1002V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R23,R24,R25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF1001V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF1001V</t>
+    <t xml:space="preserve">R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF5602V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF5602V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1,R3,R4,R6,R7,R9,R10,R12,R13,R16,R17,R20,R37,R42,R49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF1003V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF1003V</t>
   </si>
   <si>
     <t xml:space="preserve">R26</t>
@@ -337,30 +397,6 @@
     <t xml:space="preserve">667-ERJ-3EKF3303V</t>
   </si>
   <si>
-    <t xml:space="preserve">R27,R28,R29,R31,R33,R34,R35,R36,R38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF3302V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF3302V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1K5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF1501V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF1501V</t>
-  </si>
-  <si>
     <t xml:space="preserve">R43</t>
   </si>
   <si>
@@ -371,30 +407,6 @@
   </si>
   <si>
     <t xml:space="preserve">667-ERJ-3EKF4703V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R44,R47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6K8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF6801V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF6801V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1,R3,R4,R6,R7,R9,R10,R12,R13,R16,R17,R20,R37,R42,R49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF1003V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF1003V</t>
   </si>
   <si>
     <t xml:space="preserve">U1,U2,U4,U5</t>
@@ -738,13 +750,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.1"/>
@@ -801,8 +813,8 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="str">
-        <f aca="false">_xlfn.CONCAT( "SMD Parts: ", SUM(E4:E29 ), " pcs" )</f>
-        <v>SMD Parts: 85 pcs</v>
+        <f aca="false">_xlfn.CONCAT( "SMD Parts: ", SUM(E4:E30 ), " pcs" )</f>
+        <v>SMD Parts: 83 pcs</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -931,7 +943,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>31</v>
@@ -1061,7 +1073,7 @@
         <v>60</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>61</v>
@@ -1123,14 +1135,14 @@
       <c r="A16" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>78</v>
@@ -1156,7 +1168,7 @@
         <v>12</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>82</v>
@@ -1208,7 +1220,7 @@
         <v>12</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>90</v>
@@ -1253,14 +1265,14 @@
       <c r="A21" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>98</v>
@@ -1338,7 +1350,7 @@
         <v>12</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>110</v>
@@ -1372,7 +1384,7 @@
       <c r="G25" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="H25" s="4" t="s">
         <v>115</v>
       </c>
       <c r="I25" s="0" t="s">
@@ -1390,7 +1402,7 @@
         <v>12</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>118</v>
@@ -1416,7 +1428,7 @@
         <v>12</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>122</v>
@@ -1435,75 +1447,84 @@
       <c r="A28" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="G28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="E28" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="H28" s="0" t="s">
+      <c r="I28" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="C29" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="E29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="I29" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G29" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="str">
-        <f aca="false">_xlfn.CONCAT( "THT Parts: ", SUM(E31:E38 ), " pcs" )</f>
+      <c r="G30" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="str">
+        <f aca="false">_xlfn.CONCAT( "THT Parts: ", SUM(E32:E39 ), " pcs" )</f>
         <v>THT Parts: 19 pcs</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E31" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>138</v>
-      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -1513,7 +1534,7 @@
         <v>140</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G32" s="0" t="s">
         <v>141</v>
@@ -1521,41 +1542,41 @@
       <c r="H32" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="I32" s="0" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="E33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="E33" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="G33" s="0" t="s">
+      <c r="H33" s="0" t="s">
         <v>146</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="G34" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G34" s="0" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1570,15 +1591,9 @@
         <v>1</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="H35" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="I35" s="0" t="s">
+      <c r="G35" s="4" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1587,15 +1602,15 @@
         <v>155</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="G36" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G36" s="0" t="s">
         <v>73</v>
       </c>
       <c r="H36" s="0" t="s">
@@ -1610,7 +1625,7 @@
         <v>159</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>1</v>
@@ -1633,26 +1648,49 @@
         <v>163</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="G38" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>167</v>
+      <c r="G39" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A31:I31"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
#7 - Removed the -5V reference. Changed R12 to have the same effect as before with -12V (-10.8V after the rectifier).
</commit_message>
<xml_diff>
--- a/bom/schraeg_BOM.xlsx
+++ b/bom/schraeg_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="163">
   <si>
     <t xml:space="preserve">SCHRÄG, v0.2.2</t>
   </si>
@@ -112,18 +112,6 @@
     <t xml:space="preserve">603-CC0603MR9BB104</t>
   </si>
   <si>
-    <t xml:space="preserve">C18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">220n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0603KRX5R9BB22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-CC0603KRX5R9BB22</t>
-  </si>
-  <si>
     <t xml:space="preserve">C2,C4,C5,C6</t>
   </si>
   <si>
@@ -196,226 +184,211 @@
     <t xml:space="preserve">771-BZT52-C4V7X</t>
   </si>
   <si>
-    <t xml:space="preserve">D6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voltage reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT-23</t>
+    <t xml:space="preserve">D5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full bridge rectifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TO-269AA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OnSemi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MB2S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512-MB2S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1,F2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTC Fuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bourns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MF-NSMF050-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-MF-NSMF050-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R15,R30,R32,R39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor, 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF4700V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF4700V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R23,R24,R25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF1001V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF1001V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1K5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF1501V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF1501V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF1002V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF1002V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14,R40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF1502V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF1502V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF2202V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF2202V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27,R28,R29,R31,R33,R34,R35,R36,R38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF3302V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF3302V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2,R5,R19,R22,R48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF4702V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF4702V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF5602V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF5602V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1,R3,R4,R6,R7,R9,R10,R13,R16,R17,R20,R37,R42,R49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF1003V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF1003V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF2203V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF2203V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF3303V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF3303V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF4703V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF4703V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1,U2,U4,U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quad op-amp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOIC-14</t>
   </si>
   <si>
     <t xml:space="preserve">Texas Instruments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LM4040CIM3-5.0/NOPB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">926-LM4040CIM350NOPB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full bridge rectifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TO-269AA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnSemi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MB2S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">512-MB2S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F1,F2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTC Fuse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bourns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MF-NSMF050-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">652-MF-NSMF050-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R15,R30,R32,R39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor, 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">470R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF4700V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF4700V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R23,R24,R25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF1001V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF1001V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1K5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF1501V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF1501V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6K8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF6801V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF6801V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF1002V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF1002V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R14,R40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF1502V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF1502V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF2202V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF2202V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R27,R28,R29,R31,R33,R34,R35,R36,R38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF3302V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF3302V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2,R5,R19,R22,R48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF4702V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF4702V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF5602V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF5602V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1,R3,R4,R6,R7,R9,R10,R12,R13,R16,R17,R20,R37,R42,R49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF1003V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF1003V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">330K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF3303V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF3303V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">470K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3EKF4703V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3EKF4703V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1,U2,U4,U5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quad op-amp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOIC-14</t>
   </si>
   <si>
     <t xml:space="preserve">TL074CPWR</t>
@@ -546,7 +519,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -590,6 +563,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -652,7 +630,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -670,6 +648,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -750,13 +732,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.1"/>
@@ -813,8 +795,8 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="str">
-        <f aca="false">_xlfn.CONCAT( "SMD Parts: ", SUM(E4:E30 ), " pcs" )</f>
-        <v>SMD Parts: 83 pcs</v>
+        <f aca="false">_xlfn.CONCAT( "SMD Parts: ", SUM(E4:E28 ), " pcs" )</f>
+        <v>SMD Parts: 81 pcs</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -937,284 +919,287 @@
         <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="H9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>38</v>
+      <c r="G10" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>61</v>
+        <v>2</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="B14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>67</v>
+        <v>4</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="B15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="I15" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F16" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="0" t="s">
+      <c r="I18" s="0" t="s">
         <v>86</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>12</v>
@@ -1223,76 +1208,76 @@
         <v>1</v>
       </c>
       <c r="F19" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F20" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F21" s="0" t="s">
+      <c r="I21" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>12</v>
@@ -1301,76 +1286,76 @@
         <v>1</v>
       </c>
       <c r="F22" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F23" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H23" s="0" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="I23" s="0" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="B24" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F24" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I24" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>12</v>
@@ -1379,62 +1364,59 @@
         <v>1</v>
       </c>
       <c r="F25" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="I25" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F26" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I26" s="0" t="s">
         <v>118</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="E27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>123</v>
@@ -1447,84 +1429,72 @@
       <c r="A28" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>12</v>
+      <c r="B28" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>127</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>38</v>
+      <c r="G28" s="0" t="s">
+        <v>128</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>133</v>
-      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="str">
+        <f aca="false">_xlfn.CONCAT( "THT Parts: ", SUM(E30:E37 ), " pcs" )</f>
+        <v>THT Parts: 19 pcs</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B31" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="E31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="E30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="0" t="s">
+      <c r="H31" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="H30" s="0" t="s">
+      <c r="I31" s="0" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="str">
-        <f aca="false">_xlfn.CONCAT( "THT Parts: ", SUM(E32:E39 ), " pcs" )</f>
-        <v>THT Parts: 19 pcs</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -1534,163 +1504,126 @@
         <v>140</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>104</v>
       </c>
       <c r="G32" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="H32" s="0" t="s">
-        <v>142</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G33" s="0" t="s">
+      <c r="F33" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="I34" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F35" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="I35" s="0" t="s">
         <v>153</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>73</v>
+        <v>155</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="H36" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="I36" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="E37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F37" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H37" s="0" t="s">
+      <c r="H37" s="4" t="s">
         <v>161</v>
       </c>
       <c r="I37" s="0" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E39" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="I39" s="0" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A29:I29"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
BOM updated with smaller packages
</commit_message>
<xml_diff>
--- a/bom/schraeg_BOM.xlsx
+++ b/bom/schraeg_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="164">
   <si>
     <t xml:space="preserve">SCHRÄG, v0.2.2</t>
   </si>
@@ -172,16 +172,19 @@
     <t xml:space="preserve">Diode, zener</t>
   </si>
   <si>
+    <t xml:space="preserve">SOT-23-3</t>
+  </si>
+  <si>
     <t xml:space="preserve">5V</t>
   </si>
   <si>
     <t xml:space="preserve">Nexperia</t>
   </si>
   <si>
-    <t xml:space="preserve">BZT52-C4V7X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">771-BZT52-C4V7X</t>
+    <t xml:space="preserve">PLVA650A,215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">771-PLVA650A-T/R</t>
   </si>
   <si>
     <t xml:space="preserve">D5</t>
@@ -466,10 +469,10 @@
     <t xml:space="preserve">Multiturn trimmer pot</t>
   </si>
   <si>
-    <t xml:space="preserve">3296W-1-104LF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">652-3296W-1-104LF</t>
+    <t xml:space="preserve">3266Y-1-104LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-3266Y-1-104LF</t>
   </si>
   <si>
     <t xml:space="preserve">RV7</t>
@@ -478,10 +481,10 @@
     <t xml:space="preserve">5K</t>
   </si>
   <si>
-    <t xml:space="preserve">3296W-1-502LF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">652-3296W-1-502LF</t>
+    <t xml:space="preserve">3266Y-1-502LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-3266Y-1-502LF</t>
   </si>
   <si>
     <t xml:space="preserve">RV8</t>
@@ -490,10 +493,10 @@
     <t xml:space="preserve">250K</t>
   </si>
   <si>
-    <t xml:space="preserve">3296W-1-254LF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">652-3296W-1-254LF</t>
+    <t xml:space="preserve">3266Y-1-254LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-3266Y-1-254LF</t>
   </si>
   <si>
     <t xml:space="preserve">SW1,SW2,SW3</t>
@@ -725,11 +728,11 @@
   </sheetPr>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.1"/>
@@ -991,76 +994,76 @@
         <v>49</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>12</v>
@@ -1069,24 +1072,24 @@
         <v>4</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>12</v>
@@ -1095,24 +1098,24 @@
         <v>3</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>12</v>
@@ -1121,24 +1124,24 @@
         <v>1</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>12</v>
@@ -1147,24 +1150,24 @@
         <v>1</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>12</v>
@@ -1173,24 +1176,24 @@
         <v>2</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>12</v>
@@ -1199,24 +1202,24 @@
         <v>1</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>12</v>
@@ -1225,24 +1228,24 @@
         <v>9</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>12</v>
@@ -1251,24 +1254,24 @@
         <v>5</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>12</v>
@@ -1277,24 +1280,24 @@
         <v>1</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>12</v>
@@ -1303,24 +1306,24 @@
         <v>15</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>12</v>
@@ -1329,24 +1332,24 @@
         <v>1</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>12</v>
@@ -1355,24 +1358,24 @@
         <v>1</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>12</v>
@@ -1381,59 +1384,59 @@
         <v>1</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1452,162 +1455,162 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>7</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>4</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>3</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#8 - Added back the FM normalization. This time with a bit more than 1 OCT range.
</commit_message>
<xml_diff>
--- a/bom/schraeg_BOM.xlsx
+++ b/bom/schraeg_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="168">
   <si>
     <t xml:space="preserve">SCHRÄG, v0.2.2</t>
   </si>
@@ -380,6 +380,18 @@
   </si>
   <si>
     <t xml:space="preserve">667-ERJ-3EKF4703V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2M2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF2204V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF2204V</t>
   </si>
   <si>
     <t xml:space="preserve">U1,U2,U4,U5</t>
@@ -726,13 +738,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.1"/>
@@ -789,7 +801,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="str">
-        <f aca="false">_xlfn.CONCAT( "SMD Parts: ", SUM(E4:E28 ), " pcs" )</f>
+        <f aca="false">_xlfn.CONCAT( "SMD Parts: ", SUM(E4:E29 ), " pcs" )</f>
         <v>SMD Parts: 81 pcs</v>
       </c>
       <c r="B3" s="3"/>
@@ -1303,7 +1315,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>105</v>
@@ -1400,75 +1412,84 @@
       <c r="A27" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="G27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="E27" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G27" s="0" t="s">
+      <c r="I27" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="E28" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G28" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="H28" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="I28" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G28" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="str">
-        <f aca="false">_xlfn.CONCAT( "THT Parts: ", SUM(E30:E37 ), " pcs" )</f>
+      <c r="G29" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="str">
+        <f aca="false">_xlfn.CONCAT( "THT Parts: ", SUM(E31:E38 ), " pcs" )</f>
         <v>THT Parts: 19 pcs</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>134</v>
-      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
@@ -1478,7 +1499,7 @@
         <v>136</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>137</v>
@@ -1486,41 +1507,41 @@
       <c r="H31" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="I31" s="0" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="E32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="E32" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="G32" s="0" t="s">
+      <c r="H32" s="0" t="s">
         <v>142</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="G33" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" s="0" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1535,15 +1556,9 @@
         <v>1</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H34" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="I34" s="0" t="s">
+      <c r="G34" s="4" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1552,15 +1567,15 @@
         <v>151</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="G35" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35" s="0" t="s">
         <v>64</v>
       </c>
       <c r="H35" s="0" t="s">
@@ -1575,7 +1590,7 @@
         <v>155</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1</v>
@@ -1598,26 +1613,49 @@
         <v>159</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="G37" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E38" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>163</v>
+      <c r="G38" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A30:I30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
#9 - Added LED input indicator.
</commit_message>
<xml_diff>
--- a/bom/schraeg_BOM.xlsx
+++ b/bom/schraeg_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="179">
   <si>
     <t xml:space="preserve">SCHRÄG, v0.3.0</t>
   </si>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">603-CC603JRNPO8BN561</t>
   </si>
   <si>
-    <t xml:space="preserve">C19,C20,C21,C22,C23,C24,C25,C26,C27,C28</t>
+    <t xml:space="preserve">C14,C15,C19,C20,C21,C22,C23,C24,C25,C26,C27,C28</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;= 25V</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">667-EEE-FC1E220AP</t>
   </si>
   <si>
-    <t xml:space="preserve">D1,D2</t>
+    <t xml:space="preserve">D1,D2,D4</t>
   </si>
   <si>
     <t xml:space="preserve">Diode, general purpose</t>
@@ -223,7 +223,7 @@
     <t xml:space="preserve">652-MF-NSMF050-2</t>
   </si>
   <si>
-    <t xml:space="preserve">R15,R30,R32,R39</t>
+    <t xml:space="preserve">R15,R30,R32,R39,R44</t>
   </si>
   <si>
     <t xml:space="preserve">Resistor, 1%</t>
@@ -425,6 +425,39 @@
   </si>
   <si>
     <t xml:space="preserve">V2164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single op-amp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM321MFX/NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">926-LM321MFX/NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED, red, 5mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kingbright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WP483IDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-WP483IDT</t>
   </si>
   <si>
     <t xml:space="preserve">J1,J2,J3,J4,J5,J6,J7</t>
@@ -738,13 +771,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.1"/>
@@ -801,8 +834,8 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="str">
-        <f aca="false">_xlfn.CONCAT( "SMD Parts: ", SUM(E4:E29 ), " pcs" )</f>
-        <v>SMD Parts: 81 pcs</v>
+        <f aca="false">_xlfn.CONCAT( "SMD Parts: ", SUM(E4:E30 ), " pcs" )</f>
+        <v>SMD Parts: 84 pcs</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -986,7 +1019,7 @@
         <v>44</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>45</v>
@@ -1081,7 +1114,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>69</v>
@@ -1477,185 +1510,231 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="str">
-        <f aca="false">_xlfn.CONCAT( "THT Parts: ", SUM(E31:E38 ), " pcs" )</f>
-        <v>THT Parts: 19 pcs</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B30" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="E31" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G31" s="0" t="s">
+      <c r="C30" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="H31" s="0" t="s">
+      <c r="E30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="H30" s="0" t="s">
         <v>138</v>
       </c>
+      <c r="I30" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="str">
+        <f aca="false">_xlfn.CONCAT( "THT Parts: ", SUM(E32:E40 ), " pcs" )</f>
+        <v>THT Parts: 20 pcs</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="B32" s="4" t="s">
         <v>140</v>
       </c>
+      <c r="B32" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>142</v>
+      </c>
       <c r="E32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>105</v>
+        <v>7</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F34" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>150</v>
+      <c r="G34" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>105</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="G37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" s="0" t="s">
         <v>64</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>164</v>
-      </c>
       <c r="E38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E40" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>167</v>
+      <c r="G40" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A31:I31"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
#10 - Corrected rectifier orientation.
</commit_message>
<xml_diff>
--- a/bom/schraeg_BOM.xlsx
+++ b/bom/schraeg_BOM.xlsx
@@ -193,16 +193,16 @@
     <t xml:space="preserve">Full bridge rectifier</t>
   </si>
   <si>
-    <t xml:space="preserve">TO-269AA</t>
+    <t xml:space="preserve">SO-4</t>
   </si>
   <si>
     <t xml:space="preserve">OnSemi</t>
   </si>
   <si>
-    <t xml:space="preserve">MB2S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">512-MB2S</t>
+    <t xml:space="preserve">MB1S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512-MB1S</t>
   </si>
   <si>
     <t xml:space="preserve">F1,F2</t>
@@ -777,7 +777,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.1"/>

</xml_diff>

<commit_message>
Corrected PTC footprint. From 1206 to 0805
</commit_message>
<xml_diff>
--- a/bom/schraeg_BOM.xlsx
+++ b/bom/schraeg_BOM.xlsx
@@ -211,7 +211,7 @@
     <t xml:space="preserve">PTC Fuse</t>
   </si>
   <si>
-    <t xml:space="preserve">1206</t>
+    <t xml:space="preserve">0805</t>
   </si>
   <si>
     <t xml:space="preserve">Bourns</t>
@@ -448,7 +448,7 @@
     <t xml:space="preserve">LED, red, 5mm</t>
   </si>
   <si>
-    <t xml:space="preserve">T-1</t>
+    <t xml:space="preserve">T-1 3/4</t>
   </si>
   <si>
     <t xml:space="preserve">Kingbright</t>
@@ -777,7 +777,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.1"/>

</xml_diff>

<commit_message>
#13 -  Halved FM input range
</commit_message>
<xml_diff>
--- a/bom/schraeg_BOM.xlsx
+++ b/bom/schraeg_BOM.xlsx
@@ -310,7 +310,7 @@
     <t xml:space="preserve">667-ERJ-3EKF3302V</t>
   </si>
   <si>
-    <t xml:space="preserve">R2,R5,R19,R22,R48</t>
+    <t xml:space="preserve">R19,R22</t>
   </si>
   <si>
     <t xml:space="preserve">47K</t>
@@ -334,7 +334,7 @@
     <t xml:space="preserve">667-ERJ-3EKF5602V</t>
   </si>
   <si>
-    <t xml:space="preserve">R1,R3,R4,R6,R7,R9,R10,R13,R16,R17,R20,R37,R42,R49</t>
+    <t xml:space="preserve">R1,R2,R3,R4,R5,R6,R7,R9,R10,R13,R16,R17,R20,R37,R42,R48,R49</t>
   </si>
   <si>
     <t xml:space="preserve">100K</t>
@@ -777,7 +777,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.1"/>
@@ -1296,7 +1296,7 @@
         <v>12</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>97</v>
@@ -1348,7 +1348,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
#12 - Changed fuse footprint to 1206
</commit_message>
<xml_diff>
--- a/bom/schraeg_BOM.xlsx
+++ b/bom/schraeg_BOM.xlsx
@@ -211,7 +211,7 @@
     <t xml:space="preserve">PTC Fuse</t>
   </si>
   <si>
-    <t xml:space="preserve">0805</t>
+    <t xml:space="preserve">1206</t>
   </si>
   <si>
     <t xml:space="preserve">Bourns</t>
@@ -777,7 +777,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.1"/>

</xml_diff>

<commit_message>
#11 - FIX: LED indicator stage connected to the output of the input stage.
</commit_message>
<xml_diff>
--- a/bom/schraeg_BOM.xlsx
+++ b/bom/schraeg_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="183">
   <si>
     <t xml:space="preserve">SCHRÄG, v0.3.2</t>
   </si>
@@ -223,10 +223,22 @@
     <t xml:space="preserve">652-MF-NSMF050-2</t>
   </si>
   <si>
-    <t xml:space="preserve">R15,R30,R32,R39,R44</t>
+    <t xml:space="preserve">R44</t>
   </si>
   <si>
     <t xml:space="preserve">Resistor, 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3EKF2200V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-3EKF2200V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R15,R30,R32,R39</t>
   </si>
   <si>
     <t xml:space="preserve">470R</t>
@@ -771,13 +783,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.1"/>
@@ -834,7 +846,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="str">
-        <f aca="false">_xlfn.CONCAT( "SMD Parts: ", SUM(E4:E30 ), " pcs" )</f>
+        <f aca="false">_xlfn.CONCAT( "SMD Parts: ", SUM(E4:E31 ), " pcs" )</f>
         <v>SMD Parts: 84 pcs</v>
       </c>
       <c r="B3" s="3"/>
@@ -1114,7 +1126,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>69</v>
@@ -1140,7 +1152,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>73</v>
@@ -1166,7 +1178,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>77</v>
@@ -1211,14 +1223,14 @@
       <c r="A18" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>85</v>
@@ -1237,14 +1249,14 @@
       <c r="A19" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>89</v>
@@ -1270,7 +1282,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>93</v>
@@ -1296,7 +1308,7 @@
         <v>12</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>97</v>
@@ -1322,7 +1334,7 @@
         <v>12</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>101</v>
@@ -1330,7 +1342,7 @@
       <c r="G22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="0" t="s">
         <v>102</v>
       </c>
       <c r="I22" s="0" t="s">
@@ -1348,7 +1360,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>105</v>
@@ -1356,7 +1368,7 @@
       <c r="G23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="H23" s="4" t="s">
         <v>106</v>
       </c>
       <c r="I23" s="0" t="s">
@@ -1364,7 +1376,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="0" t="s">
         <v>108</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1374,7 +1386,7 @@
         <v>12</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>109</v>
@@ -1390,7 +1402,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1471,119 +1483,128 @@
       <c r="A28" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="G28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="E28" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G28" s="0" t="s">
+      <c r="I28" s="0" t="s">
         <v>127</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="E29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G29" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="H29" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="E29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="0" t="s">
+      <c r="I29" s="0" t="s">
         <v>133</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="C30" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="E30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>127</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="I30" s="0" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="str">
-        <f aca="false">_xlfn.CONCAT( "THT Parts: ", SUM(E32:E40 ), " pcs" )</f>
+      <c r="B31" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="str">
+        <f aca="false">_xlfn.CONCAT( "THT Parts: ", SUM(E33:E41 ), " pcs" )</f>
         <v>THT Parts: 20 pcs</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>145</v>
-      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="E33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="E33" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G33" s="0" t="s">
+      <c r="H33" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="H33" s="0" t="s">
+      <c r="I33" s="0" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1595,7 +1616,7 @@
         <v>151</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>152</v>
@@ -1603,41 +1624,41 @@
       <c r="H34" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="I34" s="0" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="E35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="E35" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" s="0" t="s">
+      <c r="H35" s="0" t="s">
         <v>157</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="G36" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" s="0" t="s">
         <v>161</v>
       </c>
     </row>
@@ -1652,15 +1673,9 @@
         <v>1</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H37" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="I37" s="0" t="s">
+      <c r="G37" s="4" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1669,15 +1684,15 @@
         <v>166</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="G38" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="0" t="s">
         <v>64</v>
       </c>
       <c r="H38" s="0" t="s">
@@ -1692,7 +1707,7 @@
         <v>170</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>1</v>
@@ -1715,26 +1730,49 @@
         <v>174</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="G40" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G40" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="I40" s="0" t="s">
-        <v>178</v>
+      <c r="G41" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A32:I32"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>